<commit_message>
DataDriven testing & pom.xml execution working
</commit_message>
<xml_diff>
--- a/testData/Opencart_LoginData.xlsx
+++ b/testData/Opencart_LoginData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pavan\June10batch\opencart\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\eclipse-workspace\opencart\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF8D4DD8-6540-4EB2-9E5E-6B129D395D71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9D7E570-AB72-419A-BCA4-C88051A06196}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="17589" xr2:uid="{1F2D179E-37D2-4BC0-88A9-F5C135B87DA5}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11400" xr2:uid="{1F2D179E-37D2-4BC0-88A9-F5C135B87DA5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -51,31 +51,31 @@
     <t>Lakshmi</t>
   </si>
   <si>
+    <t>laksh@yahoo.com</t>
+  </si>
+  <si>
+    <t>Laxmi</t>
+  </si>
+  <si>
+    <t>Invalid</t>
+  </si>
+  <si>
+    <t>laks@yahoo.com</t>
+  </si>
+  <si>
+    <t>xyz</t>
+  </si>
+  <si>
+    <t>pavanoltraining@gmail.com</t>
+  </si>
+  <si>
+    <t>test@123</t>
+  </si>
+  <si>
+    <t>abc123@gmail.com</t>
+  </si>
+  <si>
     <t>Valid</t>
-  </si>
-  <si>
-    <t>laksh@yahoo.com</t>
-  </si>
-  <si>
-    <t>Laxmi</t>
-  </si>
-  <si>
-    <t>Invalid</t>
-  </si>
-  <si>
-    <t>laks@yahoo.com</t>
-  </si>
-  <si>
-    <t>xyz</t>
-  </si>
-  <si>
-    <t>pavanoltraining@gmail.com</t>
-  </si>
-  <si>
-    <t>test@123</t>
-  </si>
-  <si>
-    <t>abc123@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -141,7 +141,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -153,9 +153,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -476,17 +473,17 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.15234375" customWidth="1"/>
-    <col min="2" max="2" width="17.3046875" customWidth="1"/>
-    <col min="3" max="3" width="18.15234375" customWidth="1"/>
+    <col min="1" max="1" width="27.140625" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -497,59 +494,59 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="C2" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>8</v>
-      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="B5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>